<commit_message>
Tested mobile devices and added CSS for landscape views
</commit_message>
<xml_diff>
--- a/testing/manually/TestScript.xlsx
+++ b/testing/manually/TestScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robbertbos/Documents/milestone2_are_you_a_hero/testing/manually/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF5098A-C4D3-8440-B987-83BBF670704D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6957034C-D174-1740-BA32-895ABA9190C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28240" windowHeight="16400" xr2:uid="{62264D32-ACA9-F34F-9C3B-790E56B59B53}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="51">
   <si>
     <t>Validations</t>
   </si>
@@ -432,7 +432,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="182">
     <dxf>
       <font>
         <b val="0"/>
@@ -2210,33 +2210,6 @@
         <i val="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
         <patternFill patternType="gray0625">
           <fgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
@@ -2621,6 +2594,1995 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border>
@@ -3742,8 +5704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4A729-DBFE-C143-A4AC-34C3AF8DE2B1}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="175" zoomScaleNormal="200" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="175" zoomScaleNormal="200" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="131" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3996,12 +5958,24 @@
       <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I13" s="11" t="s">
         <v>30</v>
       </c>
@@ -4016,12 +5990,24 @@
       <c r="B14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I14" s="11" t="s">
         <v>30</v>
       </c>
@@ -4036,12 +6022,24 @@
       <c r="B15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I15" s="11" t="s">
         <v>30</v>
       </c>
@@ -4056,12 +6054,24 @@
       <c r="B16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I16" s="11" t="s">
         <v>30</v>
       </c>
@@ -4076,12 +6086,24 @@
       <c r="B17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="I17" s="11" t="s">
         <v>30</v>
       </c>
@@ -4126,12 +6148,24 @@
       <c r="B20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I20" s="11" t="s">
         <v>30</v>
       </c>
@@ -4146,12 +6180,24 @@
       <c r="B21" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I21" s="11" t="s">
         <v>30</v>
       </c>
@@ -4166,12 +6212,24 @@
       <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I22" s="11" t="s">
         <v>30</v>
       </c>
@@ -4186,12 +6244,24 @@
       <c r="B23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I23" s="11" t="s">
         <v>30</v>
       </c>
@@ -4206,12 +6276,24 @@
       <c r="B24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I24" s="11" t="s">
         <v>30</v>
       </c>
@@ -4226,12 +6308,24 @@
       <c r="B25" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I25" s="11" t="s">
         <v>30</v>
       </c>
@@ -4276,12 +6370,24 @@
       <c r="B28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I28" s="11" t="s">
         <v>30</v>
       </c>
@@ -4296,12 +6402,24 @@
       <c r="B29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I29" s="11" t="s">
         <v>30</v>
       </c>
@@ -4316,12 +6434,24 @@
       <c r="B30" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="C30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I30" s="11" t="s">
         <v>30</v>
       </c>
@@ -4336,12 +6466,24 @@
       <c r="B31" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I31" s="11" t="s">
         <v>30</v>
       </c>
@@ -4356,12 +6498,24 @@
       <c r="B32" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="C32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I32" s="11" t="s">
         <v>30</v>
       </c>
@@ -4376,12 +6530,24 @@
       <c r="B33" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="C33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I33" s="11" t="s">
         <v>30</v>
       </c>
@@ -4426,12 +6592,24 @@
       <c r="B36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="C36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I36" s="11" t="s">
         <v>30</v>
       </c>
@@ -4446,12 +6624,24 @@
       <c r="B37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
+      <c r="C37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I37" s="11" t="s">
         <v>30</v>
       </c>
@@ -4466,12 +6656,24 @@
       <c r="B38" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
+      <c r="C38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I38" s="11" t="s">
         <v>30</v>
       </c>
@@ -4486,12 +6688,24 @@
       <c r="B39" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="C39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I39" s="11" t="s">
         <v>30</v>
       </c>
@@ -4506,12 +6720,24 @@
       <c r="B40" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="C40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I40" s="11" t="s">
         <v>30</v>
       </c>
@@ -4556,12 +6782,24 @@
       <c r="B43" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="C43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I43" s="11" t="s">
         <v>30</v>
       </c>
@@ -4576,12 +6814,24 @@
       <c r="B44" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
+      <c r="C44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I44" s="11" t="s">
         <v>30</v>
       </c>
@@ -4596,12 +6846,24 @@
       <c r="B45" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
+      <c r="C45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I45" s="11" t="s">
         <v>30</v>
       </c>
@@ -4616,12 +6878,24 @@
       <c r="B46" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
+      <c r="C46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I46" s="11" t="s">
         <v>30</v>
       </c>
@@ -4636,12 +6910,24 @@
       <c r="B47" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
+      <c r="C47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="I47" s="11" t="s">
         <v>30</v>
       </c>
@@ -4923,170 +7209,386 @@
     <mergeCell ref="B26:K26"/>
   </mergeCells>
   <conditionalFormatting sqref="B19:K19">
-    <cfRule type="cellIs" dxfId="109" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="280" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:I13 C14:H14 C15:I17 C9:J10">
-    <cfRule type="cellIs" dxfId="108" priority="161" operator="equal">
+  <conditionalFormatting sqref="C9:J10 I15:I17 I13 D17 C13:F16">
+    <cfRule type="cellIs" dxfId="180" priority="261" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:I13 C14:H14 C15:I17 C9:J10">
-    <cfRule type="cellIs" dxfId="107" priority="160" operator="equal">
+  <conditionalFormatting sqref="C9:J10 I15:I17 I13 D17 C13:F16">
+    <cfRule type="cellIs" dxfId="179" priority="260" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:I13 C14:H14 C15:I17 C9:J10">
-    <cfRule type="cellIs" dxfId="106" priority="158" operator="equal">
+  <conditionalFormatting sqref="C9:J10 I15:I17 I13 D17 C13:F16">
+    <cfRule type="cellIs" dxfId="178" priority="258" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="259" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:H25">
-    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
+  <conditionalFormatting sqref="I20:I25">
+    <cfRule type="cellIs" dxfId="176" priority="169" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:H25">
-    <cfRule type="cellIs" dxfId="99" priority="100" operator="equal">
+  <conditionalFormatting sqref="I20:I25">
+    <cfRule type="cellIs" dxfId="175" priority="168" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:H25">
-    <cfRule type="cellIs" dxfId="98" priority="98" operator="equal">
+  <conditionalFormatting sqref="I20:I25">
+    <cfRule type="cellIs" dxfId="174" priority="166" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="167" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:H39">
-    <cfRule type="cellIs" dxfId="96" priority="97" operator="equal">
+  <conditionalFormatting sqref="C43:E46">
+    <cfRule type="cellIs" dxfId="164" priority="193" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:H39">
-    <cfRule type="cellIs" dxfId="95" priority="96" operator="equal">
+  <conditionalFormatting sqref="C43:E46">
+    <cfRule type="cellIs" dxfId="163" priority="192" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:H39">
-    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
+  <conditionalFormatting sqref="C43:E46">
+    <cfRule type="cellIs" dxfId="162" priority="190" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="191" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:H46">
-    <cfRule type="cellIs" dxfId="92" priority="93" operator="equal">
+  <conditionalFormatting sqref="C50:H51">
+    <cfRule type="cellIs" dxfId="160" priority="189" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:H46">
-    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
+  <conditionalFormatting sqref="C50:H51">
+    <cfRule type="cellIs" dxfId="159" priority="188" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:H46">
-    <cfRule type="cellIs" dxfId="90" priority="90" operator="equal">
+  <conditionalFormatting sqref="C50:H51">
+    <cfRule type="cellIs" dxfId="158" priority="186" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="187" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:H51">
-    <cfRule type="cellIs" dxfId="88" priority="89" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="156" priority="185" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:H51">
-    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="155" priority="184" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:H51">
-    <cfRule type="cellIs" dxfId="86" priority="86" operator="equal">
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="154" priority="182" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="183" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
+  <conditionalFormatting sqref="B27:K27">
+    <cfRule type="cellIs" dxfId="152" priority="165" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36:H40">
+    <cfRule type="cellIs" dxfId="147" priority="88" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="83" priority="84" operator="equal">
+  <conditionalFormatting sqref="G36:H40">
+    <cfRule type="cellIs" dxfId="146" priority="87" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+  <conditionalFormatting sqref="G36:H40">
+    <cfRule type="cellIs" dxfId="145" priority="85" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="86" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I25">
-    <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
+  <conditionalFormatting sqref="I28:I33">
+    <cfRule type="cellIs" dxfId="143" priority="156" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I25">
-    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
+  <conditionalFormatting sqref="I28:I33">
+    <cfRule type="cellIs" dxfId="142" priority="155" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I25">
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+  <conditionalFormatting sqref="I28:I33">
+    <cfRule type="cellIs" dxfId="141" priority="153" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="154" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:K27">
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="131" priority="144" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="130" priority="143" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" dxfId="129" priority="141" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="142" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:H33">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+  <conditionalFormatting sqref="I47">
+    <cfRule type="cellIs" dxfId="119" priority="132" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:H33">
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
+  <conditionalFormatting sqref="I47">
+    <cfRule type="cellIs" dxfId="118" priority="131" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:H33">
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
+  <conditionalFormatting sqref="I47">
+    <cfRule type="cellIs" dxfId="117" priority="129" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="130" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I33">
+  <conditionalFormatting sqref="J13:J17">
+    <cfRule type="cellIs" dxfId="115" priority="128" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:J17">
+    <cfRule type="cellIs" dxfId="114" priority="127" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13:J17">
+    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:J25">
+    <cfRule type="cellIs" dxfId="111" priority="124" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:J25">
+    <cfRule type="cellIs" dxfId="110" priority="123" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:J25">
+    <cfRule type="cellIs" dxfId="109" priority="121" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="122" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:J33">
+    <cfRule type="cellIs" dxfId="107" priority="120" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:J33">
+    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:J33">
+    <cfRule type="cellIs" dxfId="105" priority="117" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="118" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:J40">
+    <cfRule type="cellIs" dxfId="103" priority="116" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:J40">
+    <cfRule type="cellIs" dxfId="102" priority="115" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:J40">
+    <cfRule type="cellIs" dxfId="101" priority="113" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="114" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43:J47">
+    <cfRule type="cellIs" dxfId="99" priority="112" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43:J47">
+    <cfRule type="cellIs" dxfId="98" priority="111" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43:J47">
+    <cfRule type="cellIs" dxfId="97" priority="109" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="110" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43:I46">
+    <cfRule type="cellIs" dxfId="95" priority="108" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43:I46">
+    <cfRule type="cellIs" dxfId="94" priority="107" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43:I46">
+    <cfRule type="cellIs" dxfId="93" priority="105" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="106" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36:I39">
+    <cfRule type="cellIs" dxfId="91" priority="104" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36:I39">
+    <cfRule type="cellIs" dxfId="90" priority="103" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36:I39">
+    <cfRule type="cellIs" dxfId="89" priority="101" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="102" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:H16">
+    <cfRule type="cellIs" dxfId="87" priority="100" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:H16">
+    <cfRule type="cellIs" dxfId="86" priority="99" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:H16">
+    <cfRule type="cellIs" dxfId="85" priority="97" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="98" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:H25">
+    <cfRule type="cellIs" dxfId="83" priority="96" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:H25">
+    <cfRule type="cellIs" dxfId="82" priority="95" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:H25">
+    <cfRule type="cellIs" dxfId="81" priority="93" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28:H33">
+    <cfRule type="cellIs" dxfId="79" priority="92" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28:H33">
+    <cfRule type="cellIs" dxfId="78" priority="91" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28:H33">
+    <cfRule type="cellIs" dxfId="77" priority="89" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="90" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43:H47">
+    <cfRule type="cellIs" dxfId="75" priority="84" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43:H47">
+    <cfRule type="cellIs" dxfId="74" priority="83" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43:H47">
+    <cfRule type="cellIs" dxfId="73" priority="81" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="82" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
     <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I33">
+  <conditionalFormatting sqref="F39">
     <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I33">
+  <conditionalFormatting sqref="F39">
     <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5094,17 +7596,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:H40">
+  <conditionalFormatting sqref="C43:F46">
     <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:H40">
+  <conditionalFormatting sqref="C43:F46">
     <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:H40">
+  <conditionalFormatting sqref="C43:F46">
     <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5112,17 +7614,35 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="E17:F17">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F17">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F17">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:F25">
     <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="D25:F25">
     <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="D25:F25">
     <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5130,17 +7650,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:H47">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:H47">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:H47">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5148,17 +7668,35 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="G17:H17">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+      <formula>$B$54</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:H17">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+      <formula>$B$55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:H17">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>$B$57</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>$B$56</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5166,17 +7704,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:J17">
+  <conditionalFormatting sqref="C20:F24">
     <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:J17">
+  <conditionalFormatting sqref="C20:F24">
     <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:J17">
+  <conditionalFormatting sqref="C20:F24">
     <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5184,17 +7722,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20:J25">
+  <conditionalFormatting sqref="C28:F32">
     <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20:J25">
+  <conditionalFormatting sqref="C28:F32">
     <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20:J25">
+  <conditionalFormatting sqref="C28:F32">
     <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5202,17 +7740,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J33">
+  <conditionalFormatting sqref="C36:F38">
     <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J33">
+  <conditionalFormatting sqref="C36:F38">
     <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J33">
+  <conditionalFormatting sqref="C36:F38">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5220,17 +7758,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:J40">
+  <conditionalFormatting sqref="C39:E39">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:J40">
+  <conditionalFormatting sqref="C39:E39">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:J40">
+  <conditionalFormatting sqref="C39:E39">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5238,17 +7776,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J43:J47">
+  <conditionalFormatting sqref="C33:F33">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J43:J47">
+  <conditionalFormatting sqref="C33:F33">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J43:J47">
+  <conditionalFormatting sqref="C33:F33">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5256,17 +7794,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43:I46">
+  <conditionalFormatting sqref="C40:F40">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43:I46">
+  <conditionalFormatting sqref="C40:F40">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43:I46">
+  <conditionalFormatting sqref="C40:F40">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5274,17 +7812,17 @@
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:I39">
+  <conditionalFormatting sqref="C47:F47">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:I39">
+  <conditionalFormatting sqref="C47:F47">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:I39">
+  <conditionalFormatting sqref="C47:F47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
@@ -5293,7 +7831,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:J33 C20:J25 C9:J10 C43:J47 C50:H51 C13:J17 C36:J40" xr:uid="{52D60307-91B2-9A4D-BABF-8A579E29AF99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36:J40 C20:J25 C9:J10 C13:J17 C50:H51 C28:J33 C43:J47" xr:uid="{52D60307-91B2-9A4D-BABF-8A579E29AF99}">
       <formula1>$B$53:$B$57</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed name background image and updated testscript
</commit_message>
<xml_diff>
--- a/testing/manually/TestScript.xlsx
+++ b/testing/manually/TestScript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robbertbos/Documents/milestone2_are_you_a_hero/testing/manually/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9D791B-63BF-4343-8D39-8101F5A9EF07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C0D54-5F65-974C-B3DD-3613627863DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="28240" windowHeight="16400" xr2:uid="{62264D32-ACA9-F34F-9C3B-790E56B59B53}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{62264D32-ACA9-F34F-9C3B-790E56B59B53}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="51">
   <si>
     <t>Validations</t>
   </si>
@@ -139,10 +139,6 @@
     <t>Poor</t>
   </si>
   <si>
-    <t>Don't have access to a 
-wider desktop</t>
-  </si>
-  <si>
     <t>JavaScript</t>
   </si>
   <si>
@@ -203,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -411,13 +407,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -427,12 +416,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="198">
+  <dxfs count="150">
     <dxf>
       <font>
         <b val="0"/>
@@ -4038,1314 +4034,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
       <border>
@@ -6140,18 +4828,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4A729-DBFE-C143-A4AC-34C3AF8DE2B1}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="175" zoomScaleNormal="200" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="200" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="131" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="4.83203125" customWidth="1"/>
     <col min="11" max="11" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6165,119 +4853,119 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="5"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="20">
       <c r="A3" s="5"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="5"/>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
       <c r="K4" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="5"/>
       <c r="B5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
+        <v>33</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
       <c r="K5" s="18"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="5"/>
       <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="18"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="5"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="20">
       <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>14</v>
@@ -6304,12 +4992,12 @@
         <v>22</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="20">
       <c r="A9" s="5"/>
       <c r="B9" s="10" t="s">
         <v>7</v>
@@ -6326,24 +5014,38 @@
       <c r="F9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="G9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="8"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="20">
       <c r="A10" s="5"/>
       <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="11" t="s">
         <v>15</v>
       </c>
@@ -6359,37 +5061,37 @@
       <c r="K10" s="11"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="5"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="5"/>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="5"/>
       <c r="B13" s="12" t="s">
         <v>10</v>
@@ -6421,10 +5123,10 @@
       <c r="K13" s="11"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="5"/>
       <c r="B14" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>30</v>
@@ -6453,10 +5155,10 @@
       <c r="K14" s="11"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="5"/>
       <c r="B15" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>30</v>
@@ -6485,7 +5187,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="5"/>
       <c r="B16" s="12" t="s">
         <v>12</v>
@@ -6517,10 +5219,10 @@
       <c r="K16" s="11"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="5"/>
       <c r="B17" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>31</v>
@@ -6549,37 +5251,37 @@
       <c r="K17" s="11"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="5"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="5"/>
-      <c r="B19" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
+      <c r="B19" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="5"/>
       <c r="B20" s="12" t="s">
         <v>10</v>
@@ -6611,10 +5313,10 @@
       <c r="K20" s="11"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="5"/>
       <c r="B21" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>30</v>
@@ -6643,10 +5345,10 @@
       <c r="K21" s="11"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="5"/>
       <c r="B22" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>30</v>
@@ -6675,10 +5377,10 @@
       <c r="K22" s="11"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="5"/>
       <c r="B23" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>30</v>
@@ -6707,7 +5409,7 @@
       <c r="K23" s="11"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="5"/>
       <c r="B24" s="12" t="s">
         <v>12</v>
@@ -6739,10 +5441,10 @@
       <c r="K24" s="11"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="5"/>
       <c r="B25" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>31</v>
@@ -6771,37 +5473,37 @@
       <c r="K25" s="11"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="5"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="5"/>
-      <c r="B27" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="B27" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="5"/>
       <c r="B28" s="12" t="s">
         <v>10</v>
@@ -6833,10 +5535,10 @@
       <c r="K28" s="11"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="5"/>
       <c r="B29" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>30</v>
@@ -6865,10 +5567,10 @@
       <c r="K29" s="11"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="5"/>
       <c r="B30" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>30</v>
@@ -6897,10 +5599,10 @@
       <c r="K30" s="11"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="5"/>
       <c r="B31" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>30</v>
@@ -6929,7 +5631,7 @@
       <c r="K31" s="11"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="5"/>
       <c r="B32" s="12" t="s">
         <v>12</v>
@@ -6961,10 +5663,10 @@
       <c r="K32" s="11"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="5"/>
       <c r="B33" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>31</v>
@@ -6993,37 +5695,37 @@
       <c r="K33" s="11"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="5"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="5"/>
-      <c r="B35" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="B35" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="5"/>
       <c r="B36" s="12" t="s">
         <v>10</v>
@@ -7055,7 +5757,7 @@
       <c r="K36" s="11"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="5"/>
       <c r="B37" s="12" t="s">
         <v>11</v>
@@ -7087,10 +5789,10 @@
       <c r="K37" s="11"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="5"/>
       <c r="B38" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>30</v>
@@ -7119,7 +5821,7 @@
       <c r="K38" s="11"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" s="5"/>
       <c r="B39" s="12" t="s">
         <v>12</v>
@@ -7151,10 +5853,10 @@
       <c r="K39" s="11"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" s="5"/>
       <c r="B40" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>31</v>
@@ -7183,37 +5885,37 @@
       <c r="K40" s="11"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="5"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="5"/>
-      <c r="B42" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
+      <c r="B42" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" s="5"/>
       <c r="B43" s="12" t="s">
         <v>10</v>
@@ -7245,7 +5947,7 @@
       <c r="K43" s="11"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" s="5"/>
       <c r="B44" s="12" t="s">
         <v>11</v>
@@ -7277,10 +5979,10 @@
       <c r="K44" s="11"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45" s="5"/>
       <c r="B45" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>30</v>
@@ -7309,7 +6011,7 @@
       <c r="K45" s="11"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="5"/>
       <c r="B46" s="12" t="s">
         <v>12</v>
@@ -7341,10 +6043,10 @@
       <c r="K46" s="11"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" s="5"/>
       <c r="B47" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>31</v>
@@ -7373,25 +6075,25 @@
       <c r="K47" s="11"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" s="5"/>
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
       <c r="K48" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="A49" s="5"/>
       <c r="B49" s="3" t="s">
         <v>14</v>
@@ -7419,7 +6121,7 @@
       <c r="K49" s="9"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="A50" s="5"/>
       <c r="B50" s="12" t="s">
         <v>12</v>
@@ -7445,11 +6147,11 @@
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" s="5"/>
       <c r="B51" s="12" t="s">
         <v>29</v>
@@ -7475,11 +6177,11 @@
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
       <c r="K51" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" hidden="1">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -7493,7 +6195,7 @@
       <c r="K52" s="8"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="16" hidden="1" customHeight="1">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -7507,7 +6209,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="16" hidden="1" customHeight="1">
       <c r="A54" s="5"/>
       <c r="B54" s="15" t="s">
         <v>30</v>
@@ -7523,7 +6225,7 @@
       <c r="K54" s="8"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="16" hidden="1" customHeight="1">
       <c r="A55" s="5"/>
       <c r="B55" s="16" t="s">
         <v>31</v>
@@ -7539,7 +6241,7 @@
       <c r="K55" s="8"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="16" hidden="1" customHeight="1">
       <c r="A56" s="5"/>
       <c r="B56" s="17" t="s">
         <v>32</v>
@@ -7555,7 +6257,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" hidden="1">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
         <v>15</v>
@@ -7571,7 +6273,7 @@
       <c r="K57" s="8"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -7585,7 +6287,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -7599,7 +6301,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -7613,7 +6315,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -7627,7 +6329,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -7641,7 +6343,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -7673,354 +6375,354 @@
     <mergeCell ref="B26:K26"/>
   </mergeCells>
   <conditionalFormatting sqref="B19:K19">
-    <cfRule type="cellIs" dxfId="197" priority="296" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="296" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:J10 I15:I17 I13 D17 C13:F16">
-    <cfRule type="cellIs" dxfId="196" priority="277" operator="equal">
+  <conditionalFormatting sqref="I15:I17 I13 D17 C13:F16 C9:J10">
+    <cfRule type="cellIs" dxfId="148" priority="277" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:J10 I15:I17 I13 D17 C13:F16">
-    <cfRule type="cellIs" dxfId="195" priority="276" operator="equal">
+  <conditionalFormatting sqref="I15:I17 I13 D17 C13:F16 C9:J10">
+    <cfRule type="cellIs" dxfId="147" priority="276" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:J10 I15:I17 I13 D17 C13:F16">
-    <cfRule type="cellIs" dxfId="194" priority="274" operator="equal">
+  <conditionalFormatting sqref="I15:I17 I13 D17 C13:F16 C9:J10">
+    <cfRule type="cellIs" dxfId="146" priority="274" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="275" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="275" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I25">
-    <cfRule type="cellIs" dxfId="192" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="185" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I25">
-    <cfRule type="cellIs" dxfId="191" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="184" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I25">
-    <cfRule type="cellIs" dxfId="190" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="182" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="183" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:E46">
-    <cfRule type="cellIs" dxfId="180" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="209" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:E46">
-    <cfRule type="cellIs" dxfId="179" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="208" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:E46">
-    <cfRule type="cellIs" dxfId="178" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="206" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="207" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="172" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="201" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="171" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="200" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="170" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="198" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="199" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:K27">
-    <cfRule type="cellIs" dxfId="168" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="181" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:H40">
-    <cfRule type="cellIs" dxfId="163" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="104" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:H40">
-    <cfRule type="cellIs" dxfId="162" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="103" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:H40">
-    <cfRule type="cellIs" dxfId="161" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="101" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="102" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I33">
-    <cfRule type="cellIs" dxfId="159" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="172" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I33">
-    <cfRule type="cellIs" dxfId="158" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="171" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I33">
-    <cfRule type="cellIs" dxfId="157" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="169" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="170" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="147" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="160" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="146" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="159" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="145" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="157" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="158" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="cellIs" dxfId="135" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="148" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="cellIs" dxfId="134" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="147" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="cellIs" dxfId="133" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="145" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="146" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:J17">
-    <cfRule type="cellIs" dxfId="131" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="144" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:J17">
-    <cfRule type="cellIs" dxfId="130" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="143" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:J17">
-    <cfRule type="cellIs" dxfId="129" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="141" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="142" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J25">
-    <cfRule type="cellIs" dxfId="127" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="140" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J25">
-    <cfRule type="cellIs" dxfId="126" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="139" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J25">
-    <cfRule type="cellIs" dxfId="125" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="137" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="138" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:J33">
-    <cfRule type="cellIs" dxfId="123" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="136" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:J33">
-    <cfRule type="cellIs" dxfId="122" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="135" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:J33">
-    <cfRule type="cellIs" dxfId="121" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="133" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="134" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J40">
-    <cfRule type="cellIs" dxfId="119" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="132" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J40">
-    <cfRule type="cellIs" dxfId="118" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="131" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J40">
-    <cfRule type="cellIs" dxfId="117" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="129" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="130" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:J47">
-    <cfRule type="cellIs" dxfId="115" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="128" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:J47">
-    <cfRule type="cellIs" dxfId="114" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="127" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:J47">
-    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="125" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="126" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:I46">
-    <cfRule type="cellIs" dxfId="111" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="124" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:I46">
-    <cfRule type="cellIs" dxfId="110" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="123" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:I46">
-    <cfRule type="cellIs" dxfId="109" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="121" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="122" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:I39">
-    <cfRule type="cellIs" dxfId="107" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="120" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:I39">
-    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="119" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:I39">
-    <cfRule type="cellIs" dxfId="105" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="117" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="118" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:H16">
-    <cfRule type="cellIs" dxfId="103" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="116" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:H16">
-    <cfRule type="cellIs" dxfId="102" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="115" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:H16">
-    <cfRule type="cellIs" dxfId="101" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="113" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="114" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:H25">
-    <cfRule type="cellIs" dxfId="99" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="112" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:H25">
-    <cfRule type="cellIs" dxfId="98" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="111" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:H25">
-    <cfRule type="cellIs" dxfId="97" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="109" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="110" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H33">
-    <cfRule type="cellIs" dxfId="95" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="108" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H33">
-    <cfRule type="cellIs" dxfId="94" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="107" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H33">
-    <cfRule type="cellIs" dxfId="93" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="105" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="106" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:H47">
-    <cfRule type="cellIs" dxfId="91" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="100" operator="equal">
       <formula>$B$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:H47">
-    <cfRule type="cellIs" dxfId="90" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="99" operator="equal">
       <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:H47">
-    <cfRule type="cellIs" dxfId="89" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="97" operator="equal">
       <formula>$B$57</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="98" operator="equal">
       <formula>$B$56</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8349,7 +7051,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36:J40 C20:J25 C9:J10 C13:J17 C43:J47 C28:J33 C50:H51" xr:uid="{52D60307-91B2-9A4D-BABF-8A579E29AF99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36:J40 C20:J25 C50:H51 C13:J17 C43:J47 C28:J33 C9:J10" xr:uid="{52D60307-91B2-9A4D-BABF-8A579E29AF99}">
       <formula1>$B$53:$B$57</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>